<commit_message>
Revert "Merge branch 'main' of https://github.com/diegoomataix/Communications-with-an-EO_Satellite-in-SSO into main"
This reverts commit 66cd837c67f2556da08953defe4f8263edefaba0, reversing
changes made to bae768ce288e49359e15c96360367cb2ab36539c.
</commit_message>
<xml_diff>
--- a/Scripts & Data/MODCODS.xlsx
+++ b/Scripts & Data/MODCODS.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31CD2B1-9E45-4757-99EF-E2636C4ED474}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="765" windowWidth="21525" windowHeight="14835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -122,7 +121,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -343,23 +342,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -395,23 +377,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -587,11 +552,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,7 +659,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="7">
-        <v>13.08</v>
+        <v>12.08</v>
       </c>
       <c r="D7" s="7">
         <v>3.28</v>

</xml_diff>

<commit_message>
Diego no me llores todo esta bien
</commit_message>
<xml_diff>
--- a/Scripts & Data/MODCODS.xlsx
+++ b/Scripts & Data/MODCODS.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6A3900-0C8E-4BE2-8CE6-0D4E8C8354BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -121,7 +122,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -148,18 +149,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -243,10 +238,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -342,6 +337,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -377,6 +389,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -552,11 +581,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,7 +688,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="7">
-        <v>12.08</v>
+        <v>13.08</v>
       </c>
       <c r="D7" s="7">
         <v>3.28</v>

</xml_diff>